<commit_message>
criando novos dados para a importação da planilha
</commit_message>
<xml_diff>
--- a/xlsx/ImportOperator.xlsx
+++ b/xlsx/ImportOperator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TG_SRRF\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98824BD-3C9A-4CFD-8BCB-85314976681C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E6E525-1E17-41F0-A9E3-A562968F7F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -554,22 +554,23 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" style="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.5703125" style="1"/>
+    <col min="9" max="16384" width="18.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -619,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -643,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -667,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -691,19 +692,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
     </row>
   </sheetData>

</xml_diff>